<commit_message>
Bugfixes in SoilWatering method regarding homing
</commit_message>
<xml_diff>
--- a/docs/pinTables.xlsx
+++ b/docs/pinTables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisw\Desktop\CA Project\CA-Project\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D512883B-946D-4FD4-8CAC-D722C68218B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13CC2035-B969-4215-A9AE-0FBB75494FB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1188,7 +1188,7 @@
   <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="92" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>